<commit_message>
add and use brigade.json
</commit_message>
<xml_diff>
--- a/monthly.xlsx
+++ b/monthly.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t xml:space="preserve">Усть-Балыкское месторождение, куст № 162 БУ «Уралмаш 5000/320 ЭК-БМЧ» зав.№ 14938</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">Пульт насосов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Внешний осмотр, проверка заземляющего проводника, проверка наличия ограждения, проверка наличия и качества смазки, проверка отсутствия посторонних шумов, чистка доступных частей от загрязнения и пыли. Протяжка контактных соединений. Опробование работы на холостом ходу и под нагрузкой.</t>
   </si>
   <si>
     <t xml:space="preserve">Система видеонаблюдения «РАСТР»</t>
@@ -228,7 +225,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -275,18 +272,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,7 +365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,10 +434,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -463,10 +444,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -496,14 +473,14 @@
   </sheetPr>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="61.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.11"/>
@@ -580,7 +557,7 @@
     </row>
     <row r="7" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -589,143 +566,143 @@
       <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="19"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="18"/>
+        <v>12</v>
+      </c>
+      <c r="E10" s="17"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="19"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="19"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="20"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="19"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="20"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -734,12 +711,12 @@
         <v>13</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -747,7 +724,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="19"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -755,111 +732,111 @@
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="20"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9"/>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="19"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="20"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9"/>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="9"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="19"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="9"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="20"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="18"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="19"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="18"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="20"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9"/>
       <c r="B34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="18"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -867,7 +844,7 @@
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="19"/>
+      <c r="E35" s="18"/>
       <c r="F35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -875,321 +852,321 @@
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="10"/>
-      <c r="E36" s="20"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="18"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="19"/>
+      <c r="E38" s="18"/>
       <c r="F38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="10"/>
-      <c r="E39" s="20"/>
+      <c r="E39" s="19"/>
       <c r="F39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9"/>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="18"/>
+      <c r="E40" s="17"/>
       <c r="F40" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="19"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="18"/>
       <c r="F41" s="14"/>
     </row>
     <row r="42" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="9"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="20"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="19"/>
       <c r="F42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="9"/>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="18"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="19"/>
+      <c r="E44" s="18"/>
       <c r="F44" s="14"/>
     </row>
     <row r="45" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="9"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="10"/>
-      <c r="E45" s="20"/>
+      <c r="E45" s="19"/>
       <c r="F45" s="16"/>
     </row>
     <row r="46" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9"/>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" s="18"/>
+      <c r="E46" s="17"/>
       <c r="F46" s="12"/>
     </row>
     <row r="47" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="9"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="10"/>
-      <c r="E47" s="19"/>
+      <c r="E47" s="18"/>
       <c r="F47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="10"/>
-      <c r="E48" s="20"/>
+      <c r="E48" s="19"/>
       <c r="F48" s="16"/>
     </row>
     <row r="49" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="9"/>
       <c r="B49" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="18"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="19"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="18"/>
       <c r="F50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="20"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="19"/>
       <c r="F51" s="16"/>
     </row>
     <row r="52" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="9"/>
-      <c r="B52" s="17" t="s">
-        <v>18</v>
+      <c r="B52" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="18"/>
+        <v>19</v>
+      </c>
+      <c r="E52" s="17"/>
       <c r="F52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="19"/>
+      <c r="E53" s="18"/>
       <c r="F53" s="14"/>
     </row>
     <row r="54" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
       <c r="D54" s="10"/>
-      <c r="E54" s="20"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="16"/>
     </row>
     <row r="55" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9"/>
-      <c r="B55" s="17" t="s">
-        <v>30</v>
+      <c r="B55" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="E55" s="17"/>
       <c r="F55" s="12"/>
     </row>
     <row r="56" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
       <c r="D56" s="10"/>
-      <c r="E56" s="19"/>
+      <c r="E56" s="18"/>
       <c r="F56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="10"/>
-      <c r="E57" s="20"/>
+      <c r="E57" s="19"/>
       <c r="F57" s="16"/>
     </row>
     <row r="58" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9"/>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="18"/>
+      <c r="E58" s="17"/>
       <c r="F58" s="12"/>
     </row>
     <row r="59" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="9"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="19"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="18"/>
       <c r="F59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="20"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="19"/>
       <c r="F60" s="16"/>
     </row>
     <row r="61" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9"/>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D61" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E61" s="18"/>
+      <c r="E61" s="17"/>
       <c r="F61" s="12"/>
     </row>
     <row r="62" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="9"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="10"/>
-      <c r="E62" s="19"/>
+      <c r="E62" s="18"/>
       <c r="F62" s="14"/>
     </row>
     <row r="63" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
       <c r="D63" s="10"/>
-      <c r="E63" s="20"/>
+      <c r="E63" s="19"/>
       <c r="F63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9"/>
       <c r="B64" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D64" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="18"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="12"/>
     </row>
     <row r="65" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="19"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="20"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="19"/>
       <c r="F66" s="16"/>
     </row>
     <row r="67" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9"/>
       <c r="B67" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E67" s="18"/>
+      <c r="E67" s="17"/>
       <c r="F67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1197,7 +1174,7 @@
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="10"/>
-      <c r="E68" s="19"/>
+      <c r="E68" s="18"/>
       <c r="F68" s="14"/>
     </row>
     <row r="69" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1205,67 +1182,67 @@
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="10"/>
-      <c r="E69" s="20"/>
+      <c r="E69" s="19"/>
       <c r="F69" s="16"/>
     </row>
     <row r="70" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="9"/>
-      <c r="B70" s="17" t="s">
-        <v>18</v>
+      <c r="B70" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C70" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E70" s="18"/>
+      <c r="E70" s="17"/>
       <c r="F70" s="12"/>
     </row>
     <row r="71" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="9"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
       <c r="D71" s="10"/>
-      <c r="E71" s="19"/>
+      <c r="E71" s="18"/>
       <c r="F71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="9"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="10"/>
-      <c r="E72" s="20"/>
+      <c r="E72" s="19"/>
       <c r="F72" s="16"/>
     </row>
     <row r="73" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="9"/>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D73" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D73" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E73" s="18"/>
+      <c r="E73" s="17"/>
       <c r="F73" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="9"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
       <c r="D74" s="10"/>
-      <c r="E74" s="19"/>
+      <c r="E74" s="18"/>
       <c r="F74" s="14"/>
     </row>
     <row r="75" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="9"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
       <c r="D75" s="10"/>
-      <c r="E75" s="20"/>
+      <c r="E75" s="19"/>
       <c r="F75" s="16"/>
     </row>
     <row r="76" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1274,12 +1251,12 @@
         <v>13</v>
       </c>
       <c r="C76" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E76" s="18"/>
+      <c r="E76" s="17"/>
       <c r="F76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1287,7 +1264,7 @@
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="10"/>
-      <c r="E77" s="19"/>
+      <c r="E77" s="18"/>
       <c r="F77" s="14"/>
     </row>
     <row r="78" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1295,51 +1272,51 @@
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="10"/>
-      <c r="E78" s="20"/>
+      <c r="E78" s="19"/>
       <c r="F78" s="16"/>
     </row>
     <row r="79" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="9"/>
-      <c r="B79" s="17" t="s">
-        <v>26</v>
+      <c r="B79" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E79" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="E79" s="17"/>
       <c r="F79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="9"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
       <c r="D80" s="10"/>
-      <c r="E80" s="19"/>
+      <c r="E80" s="18"/>
       <c r="F80" s="14"/>
     </row>
     <row r="81" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="9"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
       <c r="D81" s="10"/>
-      <c r="E81" s="20"/>
+      <c r="E81" s="19"/>
       <c r="F81" s="16"/>
     </row>
     <row r="82" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="9"/>
       <c r="B82" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C82" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D82" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E82" s="18"/>
+      <c r="E82" s="17"/>
       <c r="F82" s="12"/>
     </row>
     <row r="83" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,7 +1324,7 @@
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="10"/>
-      <c r="E83" s="19"/>
+      <c r="E83" s="18"/>
       <c r="F83" s="14"/>
     </row>
     <row r="84" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1355,21 +1332,21 @@
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="10"/>
-      <c r="E84" s="20"/>
+      <c r="E84" s="19"/>
       <c r="F84" s="16"/>
     </row>
     <row r="85" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="9"/>
       <c r="B85" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C85" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="D85" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D85" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E85" s="18"/>
+      <c r="E85" s="17"/>
       <c r="F85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1377,7 +1354,7 @@
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="10"/>
-      <c r="E86" s="19"/>
+      <c r="E86" s="18"/>
       <c r="F86" s="14"/>
     </row>
     <row r="87" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1385,67 +1362,67 @@
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="10"/>
-      <c r="E87" s="20"/>
+      <c r="E87" s="19"/>
       <c r="F87" s="16"/>
     </row>
     <row r="88" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="9"/>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C88" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D88" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E88" s="18"/>
+      <c r="E88" s="17"/>
       <c r="F88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="9"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
       <c r="D89" s="10"/>
-      <c r="E89" s="19"/>
+      <c r="E89" s="18"/>
       <c r="F89" s="14"/>
     </row>
     <row r="90" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="9"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
       <c r="D90" s="10"/>
-      <c r="E90" s="20"/>
+      <c r="E90" s="19"/>
       <c r="F90" s="16"/>
     </row>
     <row r="91" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="9"/>
-      <c r="B91" s="17" t="s">
-        <v>26</v>
+      <c r="B91" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C91" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D91" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D91" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E91" s="18"/>
+      <c r="E91" s="17"/>
       <c r="F91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="9"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="17"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
       <c r="D92" s="10"/>
-      <c r="E92" s="19"/>
+      <c r="E92" s="18"/>
       <c r="F92" s="14"/>
     </row>
     <row r="93" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="9"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="17"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
       <c r="D93" s="10"/>
-      <c r="E93" s="20"/>
+      <c r="E93" s="19"/>
       <c r="F93" s="16"/>
     </row>
     <row r="94" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1454,12 +1431,12 @@
         <v>10</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E94" s="18"/>
+        <v>63</v>
+      </c>
+      <c r="E94" s="17"/>
       <c r="F94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1467,7 +1444,7 @@
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="10"/>
-      <c r="E95" s="19"/>
+      <c r="E95" s="18"/>
       <c r="F95" s="14"/>
     </row>
     <row r="96" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1475,21 +1452,21 @@
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="10"/>
-      <c r="E96" s="20"/>
+      <c r="E96" s="19"/>
       <c r="F96" s="16"/>
     </row>
     <row r="97" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="22"/>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="23"/>
-      <c r="B98" s="23"/>
-      <c r="C98" s="23"/>
-      <c r="D98" s="23"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="23"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="128">

</xml_diff>